<commit_message>
getRoutes and getReqBody from swagger.json added
</commit_message>
<xml_diff>
--- a/testData/HyWorksData.xlsx
+++ b/testData/HyWorksData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\3D Objects\automation framework\RestAssuredAutomation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E8155E-08DD-468F-81AB-69D3BC6B752F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9139478F-A7DC-4983-8F39-DECE2A667277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="111">
   <si>
     <t>Y</t>
   </si>
@@ -324,17 +324,78 @@
   <si>
     <t>declined</t>
   </si>
+  <si>
+    <t>Routes</t>
+  </si>
+  <si>
+    <t>RouteName</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>baseUrl</t>
+  </si>
+  <si>
+    <t>https://jobify-app-api-dev.onrender.com/api/v1</t>
+  </si>
+  <si>
+    <t>/auth/register</t>
+  </si>
+  <si>
+    <t>/auth/login</t>
+  </si>
+  <si>
+    <t>/auth/user/{email}</t>
+  </si>
+  <si>
+    <t>/jobs</t>
+  </si>
+  <si>
+    <t>/jobs/{id}</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>deleteUser</t>
+  </si>
+  <si>
+    <t>createJob</t>
+  </si>
+  <si>
+    <t>getAllJobs</t>
+  </si>
+  <si>
+    <t>getSingleJob</t>
+  </si>
+  <si>
+    <t>updateJob</t>
+  </si>
+  <si>
+    <t>deleteJob</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -481,36 +542,39 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -793,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC56"/>
+  <dimension ref="A1:BC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -2270,6 +2334,95 @@
         <v>92</v>
       </c>
     </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D18" r:id="rId1" xr:uid="{E2A95F8D-6B5F-4EB1-AD9E-6446AF002933}"/>
@@ -2287,6 +2440,7 @@
     <hyperlink ref="B32" r:id="rId13" xr:uid="{9CCC5A03-4848-4F60-9F9A-A33CC174BBEB}"/>
     <hyperlink ref="B37" r:id="rId14" xr:uid="{A290E24E-1ECC-42CD-BDBA-2E654F745BC9}"/>
     <hyperlink ref="B42" r:id="rId15" xr:uid="{12FC5269-AFA4-423F-9723-4EA781F8EC07}"/>
+    <hyperlink ref="B60" r:id="rId16" xr:uid="{97E04DA2-E0BF-425D-BC23-84A54DB4D9A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>